<commit_message>
Created Avatar Inventory SQL Files
</commit_message>
<xml_diff>
--- a/database_reference.xlsx
+++ b/database_reference.xlsx
@@ -5,21 +5,22 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\beanbeanjuice\Desktop\Coding Projects\KohuCafe\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\beanbeanjuice\Desktop\Coding Projects\Java-KohuCafe-Database-Wrapper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3031992-E04E-4848-BC8E-5B3634F00EC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3454C7B5-BB74-4F2C-99B8-9A0C9B10C0EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{C208192E-A14C-4078-A5E3-4C0C87704A16}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{C208192E-A14C-4078-A5E3-4C0C87704A16}"/>
   </bookViews>
   <sheets>
     <sheet name="Reference Sheet" sheetId="1" r:id="rId1"/>
     <sheet name="avatar_items" sheetId="2" r:id="rId2"/>
-    <sheet name="avatar_statistics" sheetId="3" r:id="rId3"/>
-    <sheet name="ranks" sheetId="7" r:id="rId4"/>
-    <sheet name="user_ranks" sheetId="4" r:id="rId5"/>
-    <sheet name="users" sheetId="5" r:id="rId6"/>
-    <sheet name="warns" sheetId="6" r:id="rId7"/>
+    <sheet name="avatar_inventories" sheetId="8" r:id="rId3"/>
+    <sheet name="avatar_statistics" sheetId="3" r:id="rId4"/>
+    <sheet name="ranks" sheetId="7" r:id="rId5"/>
+    <sheet name="user_ranks" sheetId="4" r:id="rId6"/>
+    <sheet name="users" sheetId="5" r:id="rId7"/>
+    <sheet name="warns" sheetId="6" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="43">
   <si>
     <t>Type</t>
   </si>
@@ -88,9 +89,6 @@
     <t>damage</t>
   </si>
   <si>
-    <t>owner</t>
-  </si>
-  <si>
     <t>DOUBLE</t>
   </si>
   <si>
@@ -170,6 +168,9 @@
   </si>
   <si>
     <t>1005742939311452200</t>
+  </si>
+  <si>
+    <t>total</t>
   </si>
 </sst>
 </file>
@@ -392,7 +393,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -428,9 +429,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -774,7 +772,7 @@
   <dimension ref="D4:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E22" sqref="A1:XFD1048576"/>
+      <selection activeCell="F16" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -840,7 +838,7 @@
   <dimension ref="D4:J8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -849,9 +847,9 @@
     <col min="5" max="5" width="7" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="33.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="4" spans="4:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -869,13 +867,13 @@
         <v>4</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="I5" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J5" s="6" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="4:10" x14ac:dyDescent="0.25">
@@ -892,13 +890,13 @@
         <v>8</v>
       </c>
       <c r="H6" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="I6" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I6" s="1" t="s">
+      <c r="J6" s="8" t="s">
         <v>14</v>
-      </c>
-      <c r="J6" s="8" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="7" spans="4:10" x14ac:dyDescent="0.25">
@@ -909,19 +907,19 @@
         <v>11</v>
       </c>
       <c r="F7" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G7" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="G7" s="3" t="s">
-        <v>18</v>
-      </c>
       <c r="H7" s="3">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I7" s="3">
+        <v>0</v>
+      </c>
+      <c r="J7" s="9">
         <v>10000</v>
-      </c>
-      <c r="J7" s="13" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="8" spans="4:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -938,7 +936,7 @@
         <v>0</v>
       </c>
       <c r="H8" s="11" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I8" s="11" t="b">
         <v>0</v>
@@ -953,6 +951,71 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6665CEF5-1F9E-4FC8-AA28-BEBC903431FA}">
+  <dimension ref="D4:F8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="4:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="5" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D5" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D6" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D7" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F7" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="4:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D8" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="F8" s="12" t="b">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5D42D40-DB5D-4B92-A0E9-91154E1B56AD}">
   <dimension ref="D4:H8"/>
   <sheetViews>
@@ -978,13 +1041,13 @@
         <v>3</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="G5" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="H5" s="15" t="s">
-        <v>22</v>
+        <v>21</v>
+      </c>
+      <c r="G5" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="H5" s="14" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="4:8" x14ac:dyDescent="0.25">
@@ -995,13 +1058,13 @@
         <v>5</v>
       </c>
       <c r="F6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G6" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="G6" s="3" t="s">
+      <c r="H6" s="9" t="s">
         <v>20</v>
-      </c>
-      <c r="H6" s="9" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="7" spans="4:8" x14ac:dyDescent="0.25">
@@ -1043,7 +1106,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84EA6D9B-A13A-4D62-A8AD-CE2AA0A5C30D}">
   <dimension ref="D4:H8"/>
   <sheetViews>
@@ -1065,7 +1128,7 @@
       <c r="D5" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="E5" s="18" t="s">
+      <c r="E5" s="17" t="s">
         <v>3</v>
       </c>
       <c r="F5" s="5" t="s">
@@ -1082,41 +1145,41 @@
       <c r="D6" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="E6" s="19" t="s">
+      <c r="E6" s="18" t="s">
         <v>10</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>12</v>
       </c>
       <c r="H6" s="8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D7" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="E7" s="20" t="s">
+      <c r="E7" s="19" t="s">
         <v>11</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H7" s="9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="4:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D8" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="E8" s="21" t="b">
+      <c r="E8" s="20" t="b">
         <v>1</v>
       </c>
       <c r="F8" s="11" t="b">
@@ -1135,7 +1198,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7BCC904-1295-4F05-BA36-2B11E1D769B3}">
   <dimension ref="D4:F8"/>
   <sheetViews>
@@ -1171,7 +1234,7 @@
         <v>5</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7" spans="4:6" x14ac:dyDescent="0.25">
@@ -1202,7 +1265,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4318E22D-285A-4228-BC14-D81E26938269}">
   <dimension ref="D4:G8"/>
   <sheetViews>
@@ -1227,10 +1290,10 @@
         <v>3</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="4:7" x14ac:dyDescent="0.25">
@@ -1241,10 +1304,10 @@
         <v>5</v>
       </c>
       <c r="F6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G6" s="9" t="s">
         <v>24</v>
-      </c>
-      <c r="G6" s="9" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="7" spans="4:7" x14ac:dyDescent="0.25">
@@ -1254,10 +1317,10 @@
       <c r="E7" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F7" s="17">
+      <c r="F7" s="16">
         <v>100</v>
       </c>
-      <c r="G7" s="16">
+      <c r="G7" s="15">
         <v>1</v>
       </c>
     </row>
@@ -1280,7 +1343,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1E51A5C-A181-4D93-B1CA-9BAB87F3C0F2}">
   <dimension ref="D4:L8"/>
   <sheetViews>
@@ -1312,23 +1375,23 @@
       <c r="F5" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="G5" s="14" t="s">
+      <c r="G5" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="H5" s="14" t="s">
+      <c r="H5" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="I5" s="14" t="s">
+      <c r="I5" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="J5" s="14" t="s">
+      <c r="J5" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="K5" s="14" t="s">
+      <c r="K5" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="L5" s="15" t="s">
-        <v>37</v>
+      <c r="L5" s="14" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="6" spans="4:12" x14ac:dyDescent="0.25">
@@ -1342,22 +1405,22 @@
         <v>5</v>
       </c>
       <c r="G6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H6" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="H6" s="1" t="s">
+      <c r="I6" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="I6" s="1" t="s">
+      <c r="J6" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="J6" s="1" t="s">
+      <c r="K6" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="K6" s="1" t="s">
-        <v>30</v>
-      </c>
       <c r="L6" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="4:12" x14ac:dyDescent="0.25">
@@ -1371,19 +1434,19 @@
         <v>7</v>
       </c>
       <c r="G7" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="H7" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="H7" s="2" t="s">
+      <c r="I7" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="I7" s="3" t="s">
+      <c r="J7" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="J7" s="3" t="s">
+      <c r="K7" s="3" t="s">
         <v>34</v>
-      </c>
-      <c r="K7" s="3" t="s">
-        <v>35</v>
       </c>
       <c r="L7" s="9">
         <v>1</v>

</xml_diff>

<commit_message>
Created the Avatar Item Handler
</commit_message>
<xml_diff>
--- a/database_reference.xlsx
+++ b/database_reference.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\beanbeanjuice\Desktop\Coding Projects\Java-KohuCafe-Database-Wrapper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3454C7B5-BB74-4F2C-99B8-9A0C9B10C0EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF278E6D-FD83-4260-AEF3-54B34D398EFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{C208192E-A14C-4078-A5E3-4C0C87704A16}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{C208192E-A14C-4078-A5E3-4C0C87704A16}"/>
   </bookViews>
   <sheets>
     <sheet name="Reference Sheet" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="45">
   <si>
     <t>Type</t>
   </si>
@@ -171,6 +171,12 @@
   </si>
   <si>
     <t>total</t>
+  </si>
+  <si>
+    <t>image_url</t>
+  </si>
+  <si>
+    <t>https://i.rtings.com/assets/products/NNCSyYNT/keychron-c1/design-medium.jpg</t>
   </si>
 </sst>
 </file>
@@ -180,7 +186,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -208,6 +214,14 @@
       <i/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -390,10 +404,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -455,8 +470,12 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -835,10 +854,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{401649A9-B639-4BCD-BF21-4B764203CCEB}">
-  <dimension ref="D4:J8"/>
+  <dimension ref="D4:K8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -847,13 +866,14 @@
     <col min="5" max="5" width="7" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="33.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="75.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="4:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="5" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="4:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="5" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D5" s="4" t="s">
         <v>0</v>
       </c>
@@ -867,16 +887,19 @@
         <v>4</v>
       </c>
       <c r="H5" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="I5" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="I5" s="5" t="s">
+      <c r="J5" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="J5" s="6" t="s">
+      <c r="K5" s="6" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D6" s="7" t="s">
         <v>2</v>
       </c>
@@ -890,16 +913,19 @@
         <v>8</v>
       </c>
       <c r="H6" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="I6" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="I6" s="1" t="s">
+      <c r="J6" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="J6" s="8" t="s">
+      <c r="K6" s="8" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D7" s="7" t="s">
         <v>1</v>
       </c>
@@ -912,17 +938,20 @@
       <c r="G7" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="H7" s="3">
+      <c r="H7" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="I7" s="3">
         <v>-1</v>
       </c>
-      <c r="I7" s="3">
-        <v>0</v>
-      </c>
-      <c r="J7" s="9">
+      <c r="J7" s="3">
+        <v>0</v>
+      </c>
+      <c r="K7" s="9">
         <v>10000</v>
       </c>
     </row>
-    <row r="8" spans="4:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="4:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D8" s="10" t="s">
         <v>6</v>
       </c>
@@ -936,17 +965,24 @@
         <v>0</v>
       </c>
       <c r="H8" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="I8" s="11" t="b">
         <v>1</v>
       </c>
-      <c r="I8" s="11" t="b">
-        <v>0</v>
-      </c>
-      <c r="J8" s="12" t="b">
+      <c r="J8" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="K8" s="12" t="b">
         <v>0</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="H7" r:id="rId1" xr:uid="{65B59426-38F8-4286-84C3-8AB19E0CE450}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -1110,7 +1146,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84EA6D9B-A13A-4D62-A8AD-CE2AA0A5C30D}">
   <dimension ref="D4:H8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Added Experience Levels to Wrapper
</commit_message>
<xml_diff>
--- a/database_reference.xlsx
+++ b/database_reference.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\beanbeanjuice\Desktop\Coding Projects\Java-KohuCafe-Database-Wrapper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF278E6D-FD83-4260-AEF3-54B34D398EFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DD06E26-560D-4D7F-A4F8-B85771469D53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{C208192E-A14C-4078-A5E3-4C0C87704A16}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="6" xr2:uid="{C208192E-A14C-4078-A5E3-4C0C87704A16}"/>
   </bookViews>
   <sheets>
     <sheet name="Reference Sheet" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="47">
   <si>
     <t>Type</t>
   </si>
@@ -177,15 +177,18 @@
   </si>
   <si>
     <t>https://i.rtings.com/assets/products/NNCSyYNT/keychron-c1/design-medium.jpg</t>
+  </si>
+  <si>
+    <t>experience</t>
+  </si>
+  <si>
+    <t>10</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="0.0"/>
-  </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -408,7 +411,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -450,12 +453,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -856,8 +853,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{401649A9-B639-4BCD-BF21-4B764203CCEB}">
   <dimension ref="D4:K8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -938,7 +935,7 @@
       <c r="G7" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="H7" s="21" t="s">
+      <c r="H7" s="19" t="s">
         <v>44</v>
       </c>
       <c r="I7" s="3">
@@ -1053,23 +1050,24 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5D42D40-DB5D-4B92-A0E9-91154E1B56AD}">
-  <dimension ref="D4:H8"/>
+  <dimension ref="D4:I8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="4" max="4" width="14.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="4:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="5" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="4:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="5" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D5" s="4" t="s">
         <v>0</v>
       </c>
@@ -1079,14 +1077,17 @@
       <c r="F5" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="G5" s="13" t="s">
+      <c r="G5" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="H5" s="14" t="s">
+      <c r="H5" s="13" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="6" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="I5" s="14" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D6" s="7" t="s">
         <v>2</v>
       </c>
@@ -1094,33 +1095,39 @@
         <v>5</v>
       </c>
       <c r="F6" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G6" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="G6" s="3" t="s">
+      <c r="H6" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="H6" s="9" t="s">
+      <c r="I6" s="9" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D7" s="7" t="s">
         <v>1</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F7" s="3">
+      <c r="F7" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="G7" s="3">
         <v>100</v>
       </c>
-      <c r="G7" s="3">
+      <c r="H7" s="3">
         <v>10</v>
       </c>
-      <c r="H7" s="9">
+      <c r="I7" s="9">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="4:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="4:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D8" s="10" t="s">
         <v>6</v>
       </c>
@@ -1133,7 +1140,10 @@
       <c r="G8" s="11" t="b">
         <v>0</v>
       </c>
-      <c r="H8" s="12" t="b">
+      <c r="H8" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="I8" s="12" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1164,7 +1174,7 @@
       <c r="D5" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="E5" s="17" t="s">
+      <c r="E5" s="15" t="s">
         <v>3</v>
       </c>
       <c r="F5" s="5" t="s">
@@ -1181,7 +1191,7 @@
       <c r="D6" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="E6" s="18" t="s">
+      <c r="E6" s="16" t="s">
         <v>10</v>
       </c>
       <c r="F6" s="1" t="s">
@@ -1198,7 +1208,7 @@
       <c r="D7" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="E7" s="19" t="s">
+      <c r="E7" s="17" t="s">
         <v>11</v>
       </c>
       <c r="F7" s="2" t="s">
@@ -1215,7 +1225,7 @@
       <c r="D8" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="E8" s="20" t="b">
+      <c r="E8" s="18" t="b">
         <v>1</v>
       </c>
       <c r="F8" s="11" t="b">
@@ -1303,79 +1313,93 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4318E22D-285A-4228-BC14-D81E26938269}">
-  <dimension ref="D4:G8"/>
+  <dimension ref="D4:H8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="4" max="4" width="14.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="4:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="5" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="4:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="5" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D5" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="E5" s="15" t="s">
         <v>3</v>
       </c>
       <c r="F5" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="G5" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="G5" s="6" t="s">
+      <c r="H5" s="6" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D6" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="E6" s="16" t="s">
         <v>5</v>
       </c>
       <c r="F6" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G6" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G6" s="9" t="s">
+      <c r="H6" s="8" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D7" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="E7" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="F7" s="16">
+      <c r="F7" s="3">
+        <v>10</v>
+      </c>
+      <c r="G7" s="3">
         <v>100</v>
       </c>
-      <c r="G7" s="15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="4:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H7" s="9">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="8" spans="4:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D8" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="E8" s="11" t="b">
+      <c r="E8" s="18" t="b">
         <v>0</v>
       </c>
       <c r="F8" s="11" t="b">
         <v>0</v>
       </c>
-      <c r="G8" s="12" t="b">
+      <c r="G8" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="H8" s="12" t="b">
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>